<commit_message>
(feat: updated case_collector.py to include GUI and auto-scroll log)
</commit_message>
<xml_diff>
--- a/99-0thers/case_collector/1111.xlsx
+++ b/99-0thers/case_collector/1111.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" tabRatio="470" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="文档目录" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="案例清单" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="通用补充信息" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="数据应用类补充信息" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="客户清单" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="附1-客户类型总览" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="附2-解决方案体系" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="文档目录" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="案例清单" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="通用补充信息" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="数据应用类补充信息" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="客户清单" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="附1-客户类型总览" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="附2-解决方案体系" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk19805799" localSheetId="1">案例清单!#REF!</definedName>
@@ -766,7 +766,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>11</col>
@@ -784,24 +784,24 @@
       <nvPicPr>
         <cNvPr id="3" name="图片 2"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="7051675" y="314325"/>
           <a:ext cx="960755" cy="334645"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -812,7 +812,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>4</col>
@@ -830,24 +830,24 @@
       <nvPicPr>
         <cNvPr id="2" name="图片 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="4552315" y="104775"/>
           <a:ext cx="8110855" cy="5974080"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1114,7 +1114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1162,7 +1162,7 @@
     <mergeCell ref="A2:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1569,16 +1569,16 @@
     <row r="4" ht="15.15" customFormat="1" customHeight="1" s="57">
       <c r="A4" s="53" t="inlineStr">
         <is>
-          <t>企业级数据仓库迁移项目（二期）项目</t>
+          <t>xxxxxx</t>
         </is>
       </c>
       <c r="B4" s="54" t="inlineStr">
         <is>
-          <t>&lt;100</t>
+          <t>300-400</t>
         </is>
       </c>
       <c r="C4" s="54" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D4" s="54" t="inlineStr">
         <is>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="E4" s="54" t="inlineStr">
         <is>
-          <t>上海农商行</t>
+          <t>xxxx</t>
         </is>
       </c>
       <c r="F4" s="54">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="J4" s="55" t="inlineStr">
         <is>
-          <t>金融业务5E部</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="K4" s="55" t="inlineStr">
@@ -1618,88 +1618,88 @@
       </c>
       <c r="L4" s="55" t="inlineStr">
         <is>
-          <t>奚昊</t>
+          <t>xx</t>
         </is>
       </c>
       <c r="M4" s="55" t="n"/>
       <c r="N4" s="55" t="inlineStr">
         <is>
+          <t>前一个合同的设计项目包含架构、模型、管理规范，实施项目不包含咨询</t>
+        </is>
+      </c>
+      <c r="O4" s="55" t="inlineStr">
+        <is>
+          <t>数据湖、离线数据仓库、实时数据仓库</t>
+        </is>
+      </c>
+      <c r="P4" s="55" t="inlineStr">
+        <is>
+          <t>腾讯的wedata（客户自己直采）</t>
+        </is>
+      </c>
+      <c r="Q4" s="55" t="inlineStr">
+        <is>
           <t>/</t>
         </is>
       </c>
-      <c r="O4" s="55" t="inlineStr">
-        <is>
-          <t>数据迁移</t>
-        </is>
-      </c>
-      <c r="P4" s="55" t="inlineStr">
+      <c r="R4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Q4" s="55" t="inlineStr">
+      <c r="S4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="R4" s="55" t="inlineStr">
+      <c r="T4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="S4" s="55" t="inlineStr">
+      <c r="U4" s="55" t="inlineStr">
+        <is>
+          <t>wedata的数据服务模块</t>
+        </is>
+      </c>
+      <c r="V4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="T4" s="55" t="inlineStr">
+      <c r="W4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="U4" s="55" t="inlineStr">
+      <c r="X4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="V4" s="55" t="inlineStr">
+      <c r="Y4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="W4" s="55" t="inlineStr">
+      <c r="Z4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="X4" s="55" t="inlineStr">
+      <c r="AA4" s="55" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Y4" s="55" t="inlineStr">
+      <c r="AB4" s="56" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Z4" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA4" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB4" s="56" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
       <c r="AC4" s="54" t="inlineStr">
         <is>
-          <t>2023.05-2023.11</t>
+          <t>xxxxx-xxxxx</t>
         </is>
       </c>
       <c r="AD4" s="54" t="inlineStr">
@@ -1718,17 +1718,17 @@
       <c r="AG4" s="54" t="n"/>
       <c r="AH4" s="54" t="inlineStr">
         <is>
-          <t>上海</t>
+          <t>华南</t>
         </is>
       </c>
       <c r="AI4" s="54" t="inlineStr">
         <is>
-          <t>焦郁17317825496</t>
+          <t>xxxxx</t>
         </is>
       </c>
       <c r="AJ4" s="54" t="inlineStr">
         <is>
-          <t>数据迁移集成测试</t>
+          <t>/</t>
         </is>
       </c>
       <c r="AK4" s="53" t="inlineStr">
@@ -1738,1535 +1738,347 @@
       </c>
     </row>
     <row r="5" ht="15.15" customFormat="1" customHeight="1" s="57">
-      <c r="A5" s="53" t="inlineStr">
-        <is>
-          <t>上海农商行2023年度内部评级系统、风险加权资产计量系统（C模式）框架协议（2023.3.24-2024.6.30）-2023年结算</t>
-        </is>
-      </c>
-      <c r="B5" s="54" t="inlineStr">
-        <is>
-          <t>&lt;100</t>
-        </is>
-      </c>
-      <c r="C5" s="54" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D5" s="54" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="E5" s="54" t="inlineStr">
-        <is>
-          <t>上海农商银行</t>
-        </is>
-      </c>
-      <c r="F5" s="54">
-        <f>IFERROR(VLOOKUP($E5,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="54">
-        <f>IFERROR(VLOOKUP($E5,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H5" s="54">
-        <f>IFERROR(VLOOKUP($E5,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I5" s="54">
-        <f>IF(VLOOKUP($E5,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E5,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J5" s="55" t="inlineStr">
-        <is>
-          <t>风险业务1部</t>
-        </is>
-      </c>
-      <c r="K5" s="55" t="inlineStr">
-        <is>
-          <t>风险业务5部</t>
-        </is>
-      </c>
-      <c r="L5" s="55" t="inlineStr">
-        <is>
-          <t>陈亮</t>
-        </is>
-      </c>
+      <c r="A5" s="53" t="n"/>
+      <c r="B5" s="54" t="n"/>
+      <c r="C5" s="54" t="n"/>
+      <c r="D5" s="54" t="n"/>
+      <c r="E5" s="54" t="n"/>
+      <c r="F5" s="54" t="n"/>
+      <c r="G5" s="54" t="n"/>
+      <c r="H5" s="54" t="n"/>
+      <c r="I5" s="54" t="n"/>
+      <c r="J5" s="55" t="n"/>
+      <c r="K5" s="55" t="n"/>
+      <c r="L5" s="55" t="n"/>
       <c r="M5" s="55" t="n"/>
-      <c r="N5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="P5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="W5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA5" s="55" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB5" s="56" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC5" s="54" t="inlineStr">
-        <is>
-          <t>2023.07-2023.12</t>
-        </is>
-      </c>
-      <c r="AD5" s="54" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE5" s="54">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A5, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF5" s="54">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A5, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="N5" s="55" t="n"/>
+      <c r="O5" s="55" t="n"/>
+      <c r="P5" s="55" t="n"/>
+      <c r="Q5" s="55" t="n"/>
+      <c r="R5" s="55" t="n"/>
+      <c r="S5" s="55" t="n"/>
+      <c r="T5" s="55" t="n"/>
+      <c r="U5" s="55" t="n"/>
+      <c r="V5" s="55" t="n"/>
+      <c r="W5" s="55" t="n"/>
+      <c r="X5" s="55" t="n"/>
+      <c r="Y5" s="55" t="n"/>
+      <c r="Z5" s="55" t="n"/>
+      <c r="AA5" s="55" t="n"/>
+      <c r="AB5" s="56" t="n"/>
+      <c r="AC5" s="54" t="n"/>
+      <c r="AD5" s="54" t="n"/>
+      <c r="AE5" s="54" t="n"/>
+      <c r="AF5" s="54" t="n"/>
       <c r="AG5" s="54" t="n"/>
-      <c r="AH5" s="54" t="inlineStr">
-        <is>
-          <t>上海</t>
-        </is>
-      </c>
-      <c r="AI5" s="54" t="inlineStr">
-        <is>
-          <t>孙麟舔13262758110</t>
-        </is>
-      </c>
-      <c r="AJ5" s="54" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK5" s="53" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH5" s="54" t="n"/>
+      <c r="AI5" s="54" t="n"/>
+      <c r="AJ5" s="54" t="n"/>
+      <c r="AK5" s="53" t="n"/>
     </row>
     <row r="6" ht="15.15" customHeight="1" s="59">
-      <c r="A6" s="10" t="inlineStr">
-        <is>
-          <t>上海农村商业银行股份有限公司2023年度企业级数据仓库和数据模型系统增选开发维护服务（C模式）框架</t>
-        </is>
-      </c>
-      <c r="B6" s="10" t="inlineStr">
-        <is>
-          <t>200-300</t>
-        </is>
-      </c>
-      <c r="C6" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D6" s="10" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="E6" s="10" t="inlineStr">
-        <is>
-          <t>上海农商行</t>
-        </is>
-      </c>
-      <c r="F6" s="10">
-        <f>IFERROR(VLOOKUP($E6,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G6" s="10">
-        <f>IFERROR(VLOOKUP($E6,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H6" s="10">
-        <f>IFERROR(VLOOKUP($E6,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I6" s="10">
-        <f>IF(VLOOKUP($E6,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E6,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J6" s="10" t="inlineStr">
-        <is>
-          <t>金融业务5E部</t>
-        </is>
-      </c>
-      <c r="K6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L6" s="10" t="inlineStr">
-        <is>
-          <t>梅燕</t>
-        </is>
-      </c>
-      <c r="N6" s="10" t="inlineStr">
-        <is>
-          <t>数据架构咨询规划，数据模型设计</t>
-        </is>
-      </c>
-      <c r="O6" s="10" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="P6" s="10" t="inlineStr">
-        <is>
-          <t>调度平台</t>
-        </is>
-      </c>
-      <c r="Q6" s="10" t="inlineStr">
-        <is>
-          <t>数据模型管理模块</t>
-        </is>
-      </c>
-      <c r="R6" s="10" t="inlineStr">
-        <is>
-          <t>数据模型，制度流程，制度流程</t>
-        </is>
-      </c>
-      <c r="S6" s="10" t="inlineStr">
-        <is>
-          <t>统一数据集市</t>
-        </is>
-      </c>
-      <c r="T6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="W6" s="10" t="inlineStr">
-        <is>
-          <t>统一CRM</t>
-        </is>
-      </c>
-      <c r="X6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA6" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB6" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC6" s="10" t="inlineStr">
-        <is>
-          <t>2023.9-2023.12</t>
-        </is>
-      </c>
-      <c r="AD6" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE6" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A6, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF6" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A6, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A6" s="10" t="n"/>
+      <c r="B6" s="10" t="n"/>
+      <c r="C6" s="10" t="n"/>
+      <c r="D6" s="10" t="n"/>
+      <c r="E6" s="10" t="n"/>
+      <c r="F6" s="10" t="n"/>
+      <c r="G6" s="10" t="n"/>
+      <c r="H6" s="10" t="n"/>
+      <c r="I6" s="10" t="n"/>
+      <c r="J6" s="10" t="n"/>
+      <c r="K6" s="10" t="n"/>
+      <c r="L6" s="10" t="n"/>
+      <c r="N6" s="10" t="n"/>
+      <c r="O6" s="10" t="n"/>
+      <c r="P6" s="10" t="n"/>
+      <c r="Q6" s="10" t="n"/>
+      <c r="R6" s="10" t="n"/>
+      <c r="S6" s="10" t="n"/>
+      <c r="T6" s="10" t="n"/>
+      <c r="U6" s="10" t="n"/>
+      <c r="V6" s="10" t="n"/>
+      <c r="W6" s="10" t="n"/>
+      <c r="X6" s="10" t="n"/>
+      <c r="Y6" s="10" t="n"/>
+      <c r="Z6" s="10" t="n"/>
+      <c r="AA6" s="10" t="n"/>
+      <c r="AB6" s="51" t="n"/>
+      <c r="AC6" s="10" t="n"/>
+      <c r="AD6" s="10" t="n"/>
+      <c r="AE6" s="10" t="n"/>
+      <c r="AF6" s="10" t="n"/>
       <c r="AG6" s="40" t="n"/>
-      <c r="AH6" s="40" t="inlineStr">
-        <is>
-          <t>上海</t>
-        </is>
-      </c>
-      <c r="AI6" s="40" t="inlineStr">
-        <is>
-          <t>焦郁17317825496</t>
-        </is>
-      </c>
-      <c r="AJ6" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK6" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH6" s="40" t="n"/>
+      <c r="AI6" s="40" t="n"/>
+      <c r="AJ6" s="40" t="n"/>
+      <c r="AK6" s="16" t="n"/>
     </row>
     <row r="7" ht="15.15" customHeight="1" s="59">
-      <c r="A7" s="10" t="inlineStr">
-        <is>
-          <t>东亚银行标签平台</t>
-        </is>
-      </c>
-      <c r="B7" s="10" t="inlineStr">
-        <is>
-          <t>&lt;100</t>
-        </is>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D7" s="10" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="E7" s="10" t="inlineStr">
-        <is>
-          <t>东亚银行</t>
-        </is>
-      </c>
-      <c r="F7" s="10">
-        <f>IFERROR(VLOOKUP($E7,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="10">
-        <f>IFERROR(VLOOKUP($E7,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H7" s="10">
-        <f>IFERROR(VLOOKUP($E7,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I7" s="10">
-        <f>IF(VLOOKUP($E7,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E7,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J7" s="10" t="inlineStr">
-        <is>
-          <t>营销业务2部</t>
-        </is>
-      </c>
-      <c r="K7" s="10" t="inlineStr">
-        <is>
-          <t>营销业务部</t>
-        </is>
-      </c>
-      <c r="L7" s="10" t="inlineStr">
-        <is>
-          <t>樊伟</t>
-        </is>
-      </c>
-      <c r="N7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="P7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T7" s="10" t="inlineStr">
-        <is>
-          <t>标签管理平台</t>
-        </is>
-      </c>
-      <c r="U7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="W7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y7" s="52" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA7" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB7" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC7" s="10" t="inlineStr">
-        <is>
-          <t>2023.09-2024.01</t>
-        </is>
-      </c>
-      <c r="AD7" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE7" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A7, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF7" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A7, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A7" s="10" t="n"/>
+      <c r="B7" s="10" t="n"/>
+      <c r="C7" s="10" t="n"/>
+      <c r="D7" s="10" t="n"/>
+      <c r="E7" s="10" t="n"/>
+      <c r="F7" s="10" t="n"/>
+      <c r="G7" s="10" t="n"/>
+      <c r="H7" s="10" t="n"/>
+      <c r="I7" s="10" t="n"/>
+      <c r="J7" s="10" t="n"/>
+      <c r="K7" s="10" t="n"/>
+      <c r="L7" s="10" t="n"/>
+      <c r="N7" s="10" t="n"/>
+      <c r="O7" s="10" t="n"/>
+      <c r="P7" s="10" t="n"/>
+      <c r="Q7" s="10" t="n"/>
+      <c r="R7" s="10" t="n"/>
+      <c r="S7" s="10" t="n"/>
+      <c r="T7" s="10" t="n"/>
+      <c r="U7" s="10" t="n"/>
+      <c r="V7" s="10" t="n"/>
+      <c r="W7" s="10" t="n"/>
+      <c r="X7" s="10" t="n"/>
+      <c r="Y7" s="52" t="n"/>
+      <c r="Z7" s="10" t="n"/>
+      <c r="AA7" s="10" t="n"/>
+      <c r="AB7" s="51" t="n"/>
+      <c r="AC7" s="10" t="n"/>
+      <c r="AD7" s="10" t="n"/>
+      <c r="AE7" s="10" t="n"/>
+      <c r="AF7" s="10" t="n"/>
       <c r="AG7" s="40" t="n"/>
-      <c r="AH7" s="40" t="inlineStr">
-        <is>
-          <t>华南</t>
-        </is>
-      </c>
-      <c r="AI7" s="40" t="inlineStr">
-        <is>
-          <t>罗军</t>
-        </is>
-      </c>
-      <c r="AJ7" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK7" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH7" s="40" t="n"/>
+      <c r="AI7" s="40" t="n"/>
+      <c r="AJ7" s="40" t="n"/>
+      <c r="AK7" s="16" t="n"/>
     </row>
     <row r="8" ht="15.15" customHeight="1" s="59">
-      <c r="A8" s="10" t="inlineStr">
-        <is>
-          <t>东莞银行数据治理项目</t>
-        </is>
-      </c>
-      <c r="B8" s="10" t="inlineStr">
-        <is>
-          <t>&lt;100</t>
-        </is>
-      </c>
-      <c r="C8" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D8" s="10" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="E8" s="10" t="inlineStr">
-        <is>
-          <t>东莞银行</t>
-        </is>
-      </c>
-      <c r="F8" s="10">
-        <f>IFERROR(VLOOKUP($E8,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G8" s="10">
-        <f>IFERROR(VLOOKUP($E8,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H8" s="10">
-        <f>IFERROR(VLOOKUP($E8,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I8" s="10">
-        <f>IF(VLOOKUP($E8,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E8,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J8" s="10" t="inlineStr">
-        <is>
-          <t>数据资产管理部</t>
-        </is>
-      </c>
-      <c r="K8" s="10" t="inlineStr">
-        <is>
-          <t>数据资产管理1部</t>
-        </is>
-      </c>
-      <c r="L8" s="10" t="inlineStr">
-        <is>
-          <t>支文英</t>
-        </is>
-      </c>
-      <c r="N8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="P8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R8" s="10" t="inlineStr">
-        <is>
-          <t>数据标准，数据质量，元数据，数据安全，数据资产盘点，数据模型，主数据，制度流程，组织架构</t>
-        </is>
-      </c>
-      <c r="S8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="W8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA8" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB8" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC8" s="10" t="inlineStr">
-        <is>
-          <t>2023.01-2024.07</t>
-        </is>
-      </c>
-      <c r="AD8" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE8" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A8, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF8" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A8, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A8" s="10" t="n"/>
+      <c r="B8" s="10" t="n"/>
+      <c r="C8" s="10" t="n"/>
+      <c r="D8" s="10" t="n"/>
+      <c r="E8" s="10" t="n"/>
+      <c r="F8" s="10" t="n"/>
+      <c r="G8" s="10" t="n"/>
+      <c r="H8" s="10" t="n"/>
+      <c r="I8" s="10" t="n"/>
+      <c r="J8" s="10" t="n"/>
+      <c r="K8" s="10" t="n"/>
+      <c r="L8" s="10" t="n"/>
+      <c r="N8" s="10" t="n"/>
+      <c r="O8" s="10" t="n"/>
+      <c r="P8" s="10" t="n"/>
+      <c r="Q8" s="10" t="n"/>
+      <c r="R8" s="10" t="n"/>
+      <c r="S8" s="10" t="n"/>
+      <c r="T8" s="10" t="n"/>
+      <c r="U8" s="10" t="n"/>
+      <c r="V8" s="10" t="n"/>
+      <c r="W8" s="10" t="n"/>
+      <c r="X8" s="10" t="n"/>
+      <c r="Y8" s="10" t="n"/>
+      <c r="Z8" s="10" t="n"/>
+      <c r="AA8" s="10" t="n"/>
+      <c r="AB8" s="51" t="n"/>
+      <c r="AC8" s="10" t="n"/>
+      <c r="AD8" s="10" t="n"/>
+      <c r="AE8" s="10" t="n"/>
+      <c r="AF8" s="10" t="n"/>
       <c r="AG8" s="40" t="n"/>
-      <c r="AH8" s="40" t="inlineStr">
-        <is>
-          <t>华南</t>
-        </is>
-      </c>
-      <c r="AI8" s="40" t="inlineStr">
-        <is>
-          <t>钟青 13326892506</t>
-        </is>
-      </c>
-      <c r="AJ8" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK8" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH8" s="40" t="n"/>
+      <c r="AI8" s="40" t="n"/>
+      <c r="AJ8" s="40" t="n"/>
+      <c r="AK8" s="16" t="n"/>
     </row>
     <row r="9" ht="15.15" customHeight="1" s="59">
-      <c r="A9" s="10" t="inlineStr">
-        <is>
-          <t>中信财务数据治理和数据中台建设项目</t>
-        </is>
-      </c>
-      <c r="B9" s="10" t="inlineStr">
-        <is>
-          <t>300-400</t>
-        </is>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D9" s="10" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="E9" s="10" t="inlineStr">
-        <is>
-          <t>中信财务</t>
-        </is>
-      </c>
-      <c r="F9" s="10">
-        <f>IFERROR(VLOOKUP($E9,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G9" s="10">
-        <f>IFERROR(VLOOKUP($E9,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H9" s="10">
-        <f>IFERROR(VLOOKUP($E9,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I9" s="10">
-        <f>IF(VLOOKUP($E9,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E9,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J9" s="10" t="inlineStr">
-        <is>
-          <t>金融业务9E部</t>
-        </is>
-      </c>
-      <c r="K9" s="10" t="inlineStr">
-        <is>
-          <t>数据资产管理2部</t>
-        </is>
-      </c>
-      <c r="L9" s="10" t="inlineStr">
-        <is>
-          <t>张悦</t>
-        </is>
-      </c>
-      <c r="N9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O9" s="10" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="P9" s="10" t="inlineStr">
-        <is>
-          <t>数据交换平台，调度平台，数据补录平台</t>
-        </is>
-      </c>
-      <c r="Q9" s="10" t="inlineStr">
-        <is>
-          <t>数据标准管理模块，元数据管理模块，数据质量管理模块，数据资产管理模块</t>
-        </is>
-      </c>
-      <c r="R9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S9" s="10" t="inlineStr">
-        <is>
-          <t>经营分析集市</t>
-        </is>
-      </c>
-      <c r="T9" s="10" t="inlineStr">
-        <is>
-          <t>指标梳理，指标库</t>
-        </is>
-      </c>
-      <c r="U9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V9" s="10" t="inlineStr">
-        <is>
-          <t>PC端管理驾驶舱，报表平台</t>
-        </is>
-      </c>
-      <c r="W9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA9" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB9" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC9" s="10" t="inlineStr">
-        <is>
-          <t>2023.08-2024.03</t>
-        </is>
-      </c>
-      <c r="AD9" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE9" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A9, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF9" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A9, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A9" s="10" t="n"/>
+      <c r="B9" s="10" t="n"/>
+      <c r="C9" s="10" t="n"/>
+      <c r="D9" s="10" t="n"/>
+      <c r="E9" s="10" t="n"/>
+      <c r="F9" s="10" t="n"/>
+      <c r="G9" s="10" t="n"/>
+      <c r="H9" s="10" t="n"/>
+      <c r="I9" s="10" t="n"/>
+      <c r="J9" s="10" t="n"/>
+      <c r="K9" s="10" t="n"/>
+      <c r="L9" s="10" t="n"/>
+      <c r="N9" s="10" t="n"/>
+      <c r="O9" s="10" t="n"/>
+      <c r="P9" s="10" t="n"/>
+      <c r="Q9" s="10" t="n"/>
+      <c r="R9" s="10" t="n"/>
+      <c r="S9" s="10" t="n"/>
+      <c r="T9" s="10" t="n"/>
+      <c r="U9" s="10" t="n"/>
+      <c r="V9" s="10" t="n"/>
+      <c r="W9" s="10" t="n"/>
+      <c r="X9" s="10" t="n"/>
+      <c r="Y9" s="10" t="n"/>
+      <c r="Z9" s="10" t="n"/>
+      <c r="AA9" s="10" t="n"/>
+      <c r="AB9" s="51" t="n"/>
+      <c r="AC9" s="10" t="n"/>
+      <c r="AD9" s="10" t="n"/>
+      <c r="AE9" s="10" t="n"/>
+      <c r="AF9" s="10" t="n"/>
       <c r="AG9" s="40" t="n"/>
-      <c r="AH9" s="40" t="inlineStr">
-        <is>
-          <t>北京</t>
-        </is>
-      </c>
-      <c r="AI9" s="40" t="inlineStr">
-        <is>
-          <t>王心成15086982266</t>
-        </is>
-      </c>
-      <c r="AJ9" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK9" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH9" s="40" t="n"/>
+      <c r="AI9" s="40" t="n"/>
+      <c r="AJ9" s="40" t="n"/>
+      <c r="AK9" s="16" t="n"/>
     </row>
     <row r="10" ht="15.15" customHeight="1" s="59">
-      <c r="A10" s="10" t="inlineStr">
-        <is>
-          <t>中化财务数据平台2023年优化升级项目</t>
-        </is>
-      </c>
-      <c r="B10" s="10" t="inlineStr">
-        <is>
-          <t>&lt;100</t>
-        </is>
-      </c>
-      <c r="C10" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D10" s="10" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="E10" s="10" t="inlineStr">
-        <is>
-          <t>中化财务</t>
-        </is>
-      </c>
-      <c r="F10" s="10">
-        <f>IFERROR(VLOOKUP($E10,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G10" s="10">
-        <f>IFERROR(VLOOKUP($E10,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H10" s="10">
-        <f>IFERROR(VLOOKUP($E10,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I10" s="10">
-        <f>IF(VLOOKUP($E10,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E10,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J10" s="10" t="inlineStr">
-        <is>
-          <t>金融业务9E部</t>
-        </is>
-      </c>
-      <c r="K10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L10" s="10" t="inlineStr">
-        <is>
-          <t>孙迎鹏</t>
-        </is>
-      </c>
-      <c r="N10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O10" s="10" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="P10" s="10" t="inlineStr">
-        <is>
-          <t>调度平台</t>
-        </is>
-      </c>
-      <c r="Q10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S10" s="10" t="inlineStr">
-        <is>
-          <t>监管集市</t>
-        </is>
-      </c>
-      <c r="T10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V10" s="10" t="inlineStr">
-        <is>
-          <t>报表平台</t>
-        </is>
-      </c>
-      <c r="W10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y10" s="10" t="inlineStr">
-        <is>
-          <t>统一监管报送，1104，人行金融统计报送（大集中），人行利率报送，EAST</t>
-        </is>
-      </c>
-      <c r="Z10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA10" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB10" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC10" s="10" t="inlineStr">
-        <is>
-          <t>2023.08-2024.03</t>
-        </is>
-      </c>
-      <c r="AD10" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE10" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A10, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF10" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A10, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A10" s="10" t="n"/>
+      <c r="B10" s="10" t="n"/>
+      <c r="C10" s="10" t="n"/>
+      <c r="D10" s="10" t="n"/>
+      <c r="E10" s="10" t="n"/>
+      <c r="F10" s="10" t="n"/>
+      <c r="G10" s="10" t="n"/>
+      <c r="H10" s="10" t="n"/>
+      <c r="I10" s="10" t="n"/>
+      <c r="J10" s="10" t="n"/>
+      <c r="K10" s="10" t="n"/>
+      <c r="L10" s="10" t="n"/>
+      <c r="N10" s="10" t="n"/>
+      <c r="O10" s="10" t="n"/>
+      <c r="P10" s="10" t="n"/>
+      <c r="Q10" s="10" t="n"/>
+      <c r="R10" s="10" t="n"/>
+      <c r="S10" s="10" t="n"/>
+      <c r="T10" s="10" t="n"/>
+      <c r="U10" s="10" t="n"/>
+      <c r="V10" s="10" t="n"/>
+      <c r="W10" s="10" t="n"/>
+      <c r="X10" s="10" t="n"/>
+      <c r="Y10" s="10" t="n"/>
+      <c r="Z10" s="10" t="n"/>
+      <c r="AA10" s="10" t="n"/>
+      <c r="AB10" s="51" t="n"/>
+      <c r="AC10" s="10" t="n"/>
+      <c r="AD10" s="10" t="n"/>
+      <c r="AE10" s="10" t="n"/>
+      <c r="AF10" s="10" t="n"/>
       <c r="AG10" s="40" t="n"/>
-      <c r="AH10" s="40" t="inlineStr">
-        <is>
-          <t>北京</t>
-        </is>
-      </c>
-      <c r="AI10" s="40" t="inlineStr">
-        <is>
-          <t>付鹏飞18911998594</t>
-        </is>
-      </c>
-      <c r="AJ10" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK10" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH10" s="40" t="n"/>
+      <c r="AI10" s="40" t="n"/>
+      <c r="AJ10" s="40" t="n"/>
+      <c r="AK10" s="16" t="n"/>
     </row>
     <row r="11" ht="15.15" customHeight="1" s="59">
-      <c r="A11" s="10" t="inlineStr">
-        <is>
-          <t>中国银行应用软件支持服务（MUREX）项目</t>
-        </is>
-      </c>
-      <c r="B11" s="10" t="inlineStr">
-        <is>
-          <t>300-400</t>
-        </is>
-      </c>
-      <c r="C11" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D11" s="10" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="E11" s="10" t="inlineStr">
-        <is>
-          <t>中国银行</t>
-        </is>
-      </c>
-      <c r="F11" s="10">
-        <f>IFERROR(VLOOKUP($E11,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="10">
-        <f>IFERROR(VLOOKUP($E11,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H11" s="10">
-        <f>IFERROR(VLOOKUP($E11,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I11" s="10">
-        <f>IF(VLOOKUP($E11,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E11,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J11" s="10" t="inlineStr">
-        <is>
-          <t>资金业务部</t>
-        </is>
-      </c>
-      <c r="K11" s="10" t="inlineStr">
-        <is>
-          <t>资金业务1部</t>
-        </is>
-      </c>
-      <c r="L11" s="10" t="inlineStr">
-        <is>
-          <t>康众</t>
-        </is>
-      </c>
-      <c r="N11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="P11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="W11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y11" s="52" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z11" s="10" t="inlineStr">
-        <is>
-          <t>资金管理系统</t>
-        </is>
-      </c>
-      <c r="AA11" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB11" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC11" s="10" t="inlineStr">
-        <is>
-          <t>2023.09-2024.06</t>
-        </is>
-      </c>
-      <c r="AD11" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE11" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A11, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF11" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A11, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A11" s="10" t="n"/>
+      <c r="B11" s="10" t="n"/>
+      <c r="C11" s="10" t="n"/>
+      <c r="D11" s="10" t="n"/>
+      <c r="E11" s="10" t="n"/>
+      <c r="F11" s="10" t="n"/>
+      <c r="G11" s="10" t="n"/>
+      <c r="H11" s="10" t="n"/>
+      <c r="I11" s="10" t="n"/>
+      <c r="J11" s="10" t="n"/>
+      <c r="K11" s="10" t="n"/>
+      <c r="L11" s="10" t="n"/>
+      <c r="N11" s="10" t="n"/>
+      <c r="O11" s="10" t="n"/>
+      <c r="P11" s="10" t="n"/>
+      <c r="Q11" s="10" t="n"/>
+      <c r="R11" s="10" t="n"/>
+      <c r="S11" s="10" t="n"/>
+      <c r="T11" s="10" t="n"/>
+      <c r="U11" s="10" t="n"/>
+      <c r="V11" s="10" t="n"/>
+      <c r="W11" s="10" t="n"/>
+      <c r="X11" s="10" t="n"/>
+      <c r="Y11" s="52" t="n"/>
+      <c r="Z11" s="10" t="n"/>
+      <c r="AA11" s="10" t="n"/>
+      <c r="AB11" s="51" t="n"/>
+      <c r="AC11" s="10" t="n"/>
+      <c r="AD11" s="10" t="n"/>
+      <c r="AE11" s="10" t="n"/>
+      <c r="AF11" s="10" t="n"/>
       <c r="AG11" s="40" t="n"/>
-      <c r="AH11" s="40" t="inlineStr">
-        <is>
-          <t>北京</t>
-        </is>
-      </c>
-      <c r="AI11" s="40" t="inlineStr">
-        <is>
-          <t>谷鑫虎15311932639</t>
-        </is>
-      </c>
-      <c r="AJ11" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK11" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH11" s="40" t="n"/>
+      <c r="AI11" s="40" t="n"/>
+      <c r="AJ11" s="40" t="n"/>
+      <c r="AK11" s="16" t="n"/>
     </row>
     <row r="12" ht="15.15" customHeight="1" s="59">
-      <c r="A12" s="10" t="inlineStr">
-        <is>
-          <t>中国银行股份有限公司银行卡数据运营服务项目</t>
-        </is>
-      </c>
-      <c r="B12" s="10" t="inlineStr">
-        <is>
-          <t>400-500</t>
-        </is>
-      </c>
-      <c r="C12" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D12" s="10" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="E12" s="10" t="inlineStr">
-        <is>
-          <t>中国银行卡中心</t>
-        </is>
-      </c>
-      <c r="F12" s="10">
-        <f>IFERROR(VLOOKUP($E12,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G12" s="10">
-        <f>IFERROR(VLOOKUP($E12,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H12" s="10">
-        <f>IFERROR(VLOOKUP($E12,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I12" s="10">
-        <f>IF(VLOOKUP($E12,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E12,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J12" s="10" t="inlineStr">
-        <is>
-          <t>咨询业务2A部</t>
-        </is>
-      </c>
-      <c r="K12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L12" s="10" t="inlineStr">
-        <is>
-          <t>贾浩</t>
-        </is>
-      </c>
-      <c r="N12" s="10" t="inlineStr">
-        <is>
-          <t>数据架构咨询规划</t>
-        </is>
-      </c>
-      <c r="O12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="P12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="W12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="X12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA12" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB12" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC12" s="10" t="inlineStr">
-        <is>
-          <t>2023.08-2024.08</t>
-        </is>
-      </c>
-      <c r="AD12" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE12" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A12, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF12" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A12, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="10" t="n"/>
+      <c r="C12" s="10" t="n"/>
+      <c r="D12" s="10" t="n"/>
+      <c r="E12" s="10" t="n"/>
+      <c r="F12" s="10" t="n"/>
+      <c r="G12" s="10" t="n"/>
+      <c r="H12" s="10" t="n"/>
+      <c r="I12" s="10" t="n"/>
+      <c r="J12" s="10" t="n"/>
+      <c r="K12" s="10" t="n"/>
+      <c r="L12" s="10" t="n"/>
+      <c r="N12" s="10" t="n"/>
+      <c r="O12" s="10" t="n"/>
+      <c r="P12" s="10" t="n"/>
+      <c r="Q12" s="10" t="n"/>
+      <c r="R12" s="10" t="n"/>
+      <c r="S12" s="10" t="n"/>
+      <c r="T12" s="10" t="n"/>
+      <c r="U12" s="10" t="n"/>
+      <c r="V12" s="10" t="n"/>
+      <c r="W12" s="10" t="n"/>
+      <c r="X12" s="10" t="n"/>
+      <c r="Y12" s="10" t="n"/>
+      <c r="Z12" s="10" t="n"/>
+      <c r="AA12" s="10" t="n"/>
+      <c r="AB12" s="51" t="n"/>
+      <c r="AC12" s="10" t="n"/>
+      <c r="AD12" s="10" t="n"/>
+      <c r="AE12" s="10" t="n"/>
+      <c r="AF12" s="10" t="n"/>
       <c r="AG12" s="40" t="n"/>
-      <c r="AH12" s="40" t="inlineStr">
-        <is>
-          <t>北京</t>
-        </is>
-      </c>
-      <c r="AI12" s="40" t="inlineStr">
-        <is>
-          <t>李莹 010-66595670</t>
-        </is>
-      </c>
-      <c r="AJ12" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK12" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH12" s="40" t="n"/>
+      <c r="AI12" s="40" t="n"/>
+      <c r="AJ12" s="40" t="n"/>
+      <c r="AK12" s="16" t="n"/>
     </row>
     <row r="13" ht="15.15" customHeight="1" s="59">
-      <c r="A13" s="10" t="inlineStr">
-        <is>
-          <t>红塔银行数据中台项目</t>
-        </is>
-      </c>
-      <c r="B13" s="10" t="inlineStr">
-        <is>
-          <t>100-200</t>
-        </is>
-      </c>
-      <c r="C13" s="10" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="E13" s="10" t="inlineStr">
-        <is>
-          <t>红塔银行</t>
-        </is>
-      </c>
-      <c r="F13" s="10">
-        <f>IFERROR(VLOOKUP($E13,客户清单!B:G,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G13" s="10">
-        <f>IFERROR(VLOOKUP($E13,客户清单!B:G,3,0),"")</f>
-        <v/>
-      </c>
-      <c r="H13" s="10">
-        <f>IFERROR(VLOOKUP($E13,客户清单!B:G,4,0),"")</f>
-        <v/>
-      </c>
-      <c r="I13" s="10">
-        <f>IF(VLOOKUP($E13,客户清单!B:G,6,0)=0,"&lt;暂未更新&gt;",VLOOKUP($E13,客户清单!B:G,6,0))</f>
-        <v/>
-      </c>
-      <c r="J13" s="10" t="inlineStr">
-        <is>
-          <t>金融交付3E</t>
-        </is>
-      </c>
-      <c r="K13" s="10" t="inlineStr">
-        <is>
-          <t>金融交付3部</t>
-        </is>
-      </c>
-      <c r="L13" s="10" t="inlineStr">
-        <is>
-          <t>刘刚</t>
-        </is>
-      </c>
-      <c r="N13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="O13" s="10" t="inlineStr">
-        <is>
-          <t>数据仓库，实时数据平台，数据湖，数仓迁移</t>
-        </is>
-      </c>
-      <c r="P13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S13" s="10" t="inlineStr">
-        <is>
-          <t>报表集市，监管集市</t>
-        </is>
-      </c>
-      <c r="T13" s="10" t="inlineStr">
-        <is>
-          <t>指标管理平台，标签管理平台，指标梳理，标签梳理、指标库、标签库</t>
-        </is>
-      </c>
-      <c r="U13" s="10" t="inlineStr">
-        <is>
-          <t>数据服务平台</t>
-        </is>
-      </c>
-      <c r="V13" s="10" t="inlineStr">
-        <is>
-          <t>自助分析，PC端管理驾驶舱，报表平台</t>
-        </is>
-      </c>
-      <c r="W13" s="10" t="inlineStr">
-        <is>
-          <t>客户画像，营销平台</t>
-        </is>
-      </c>
-      <c r="X13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Y13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Z13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AA13" s="10" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AB13" s="51" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AC13" s="10" t="inlineStr">
-        <is>
-          <t>2023.10-2024.12</t>
-        </is>
-      </c>
-      <c r="AD13" s="10" t="inlineStr">
-        <is>
-          <t>实施中</t>
-        </is>
-      </c>
-      <c r="AE13" s="10">
-        <f>IFERROR(HYPERLINK("#'通用补充信息'!A"&amp;MATCH(A13, 通用补充信息!A:A, 0), "&gt;&gt;&gt;通用补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
-      <c r="AF13" s="10">
-        <f>IFERROR(HYPERLINK("#'数据应用类补充信息'!A"&amp;MATCH(A13, 数据应用类补充信息!A:A, 0), "&gt;&gt;&gt;数据应用类补充信息&lt;&lt;&lt;"), "&gt;&gt;&gt;暂无补充&lt;&lt;&lt;")</f>
-        <v/>
-      </c>
+      <c r="A13" s="10" t="n"/>
+      <c r="B13" s="10" t="n"/>
+      <c r="C13" s="10" t="n"/>
+      <c r="D13" s="10" t="n"/>
+      <c r="E13" s="10" t="n"/>
+      <c r="F13" s="10" t="n"/>
+      <c r="G13" s="10" t="n"/>
+      <c r="H13" s="10" t="n"/>
+      <c r="I13" s="10" t="n"/>
+      <c r="J13" s="10" t="n"/>
+      <c r="K13" s="10" t="n"/>
+      <c r="L13" s="10" t="n"/>
+      <c r="N13" s="10" t="n"/>
+      <c r="O13" s="10" t="n"/>
+      <c r="P13" s="10" t="n"/>
+      <c r="Q13" s="10" t="n"/>
+      <c r="R13" s="10" t="n"/>
+      <c r="S13" s="10" t="n"/>
+      <c r="T13" s="10" t="n"/>
+      <c r="U13" s="10" t="n"/>
+      <c r="V13" s="10" t="n"/>
+      <c r="W13" s="10" t="n"/>
+      <c r="X13" s="10" t="n"/>
+      <c r="Y13" s="10" t="n"/>
+      <c r="Z13" s="10" t="n"/>
+      <c r="AA13" s="10" t="n"/>
+      <c r="AB13" s="51" t="n"/>
+      <c r="AC13" s="10" t="n"/>
+      <c r="AD13" s="10" t="n"/>
+      <c r="AE13" s="10" t="n"/>
+      <c r="AF13" s="10" t="n"/>
       <c r="AG13" s="40" t="n"/>
-      <c r="AH13" s="40" t="inlineStr">
-        <is>
-          <t>西南</t>
-        </is>
-      </c>
-      <c r="AI13" s="40" t="inlineStr">
-        <is>
-          <t>梁红兵13577702763</t>
-        </is>
-      </c>
-      <c r="AJ13" s="40" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="AK13" s="16" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="AH13" s="40" t="n"/>
+      <c r="AI13" s="40" t="n"/>
+      <c r="AJ13" s="40" t="n"/>
+      <c r="AK13" s="16" t="n"/>
     </row>
     <row r="14" ht="15.15" customHeight="1" s="59">
       <c r="A14" s="10" t="n"/>
@@ -4248,23 +3060,23 @@
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="AI1:AI3"/>
-    <mergeCell ref="AJ1:AJ3"/>
-    <mergeCell ref="AK1:AK3"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:I2"/>
-    <mergeCell ref="AE1:AF2"/>
-    <mergeCell ref="AG1:AH2"/>
-    <mergeCell ref="J1:L2"/>
-    <mergeCell ref="AB1:AD2"/>
-    <mergeCell ref="M1:AA1"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="J1:L2"/>
+    <mergeCell ref="AK1:AK3"/>
+    <mergeCell ref="AG1:AH2"/>
+    <mergeCell ref="AE1:AF2"/>
+    <mergeCell ref="AB1:AD2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AJ1:AJ3"/>
+    <mergeCell ref="E1:I2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="M1:AA1"/>
     <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="AD3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="AD3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"已完成,实施中"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4467,21 +3279,23 @@
     <row r="4" ht="15" customFormat="1" customHeight="1" s="31">
       <c r="A4" s="14" t="inlineStr">
         <is>
-          <t>企业级数据仓库迁移项目（二期）项目</t>
+          <t>xxxxxx</t>
         </is>
       </c>
       <c r="B4" s="14" t="inlineStr">
         <is>
-          <t>大数据</t>
+          <t>xxxx1</t>
         </is>
       </c>
       <c r="C4" s="14" t="inlineStr">
         <is>
-          <t>CDP7.1.7</t>
-        </is>
-      </c>
-      <c r="D4" s="14" t="n">
-        <v>27</v>
+          <t>xx</t>
+        </is>
+      </c>
+      <c r="D4" s="14" t="inlineStr">
+        <is>
+          <t>xxxx</t>
+        </is>
       </c>
       <c r="E4" s="14" t="inlineStr">
         <is>
@@ -4495,37 +3309,37 @@
       </c>
       <c r="G4" s="14" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>xxxxx</t>
         </is>
       </c>
       <c r="H4" s="14" t="inlineStr">
         <is>
-          <t>大数据平台开发IDE(致宇)</t>
+          <t>xx</t>
         </is>
       </c>
       <c r="I4" s="14" t="inlineStr">
         <is>
+          <t>xxx</t>
+        </is>
+      </c>
+      <c r="J4" s="14" t="inlineStr">
+        <is>
           <t>/</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr">
+      <c r="K4" s="14" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
       <c r="L4" s="14" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="M4" s="14" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>xxxxx-xxxxx</t>
         </is>
       </c>
       <c r="N4" s="14" t="inlineStr">
@@ -4536,12 +3350,12 @@
       <c r="O4" s="14" t="n"/>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>监管报送，管理驾驶舱</t>
+          <t>/</t>
         </is>
       </c>
       <c r="Q4" s="14" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>/</t>
         </is>
       </c>
       <c r="R4" s="14" t="inlineStr">
@@ -4551,986 +3365,240 @@
       </c>
       <c r="S4" s="14" t="inlineStr">
         <is>
-          <t>CDP</t>
+          <t>GuassDWS</t>
         </is>
       </c>
       <c r="T4" s="16" t="inlineStr">
         <is>
-          <t>2022.09-2024.04</t>
+          <t>2020.07-2024/11</t>
         </is>
       </c>
       <c r="U4" s="16" t="inlineStr">
         <is>
-          <t>新老并行验证</t>
+          <t>需求分析</t>
         </is>
       </c>
       <c r="V4" s="14" t="inlineStr">
         <is>
-          <t>否</t>
+          <t>/</t>
         </is>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="59">
-      <c r="A5" s="13" t="inlineStr">
-        <is>
-          <t>上海农商行2023年度内部评级系统、风险加权资产计量系统（C模式）框架协议（2023.3.24-2024.6.30）-2023年结算</t>
-        </is>
-      </c>
-      <c r="B5" s="13" t="inlineStr">
-        <is>
-          <t>ORACLE</t>
-        </is>
-      </c>
-      <c r="C5" s="13" t="inlineStr">
-        <is>
-          <t>19c</t>
-        </is>
-      </c>
-      <c r="D5" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="H5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M5" s="13" t="inlineStr">
-        <is>
-          <t>Redhat7.7</t>
-        </is>
-      </c>
-      <c r="N5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A5" s="13" t="n"/>
+      <c r="B5" s="13" t="n"/>
+      <c r="C5" s="13" t="n"/>
+      <c r="D5" s="13" t="n"/>
+      <c r="E5" s="13" t="n"/>
+      <c r="F5" s="13" t="n"/>
+      <c r="G5" s="13" t="n"/>
+      <c r="H5" s="13" t="n"/>
+      <c r="I5" s="13" t="n"/>
+      <c r="J5" s="13" t="n"/>
+      <c r="K5" s="13" t="n"/>
+      <c r="L5" s="13" t="n"/>
+      <c r="M5" s="13" t="n"/>
+      <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
-      <c r="P5" s="13" t="inlineStr">
-        <is>
-          <t>对公授信，个人贷款</t>
-        </is>
-      </c>
-      <c r="Q5" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R5" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="S5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U5" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V5" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="P5" s="13" t="n"/>
+      <c r="Q5" s="13" t="n"/>
+      <c r="R5" s="13" t="n"/>
+      <c r="S5" s="13" t="n"/>
+      <c r="T5" s="13" t="n"/>
+      <c r="U5" s="13" t="n"/>
+      <c r="V5" s="13" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1" s="59">
-      <c r="A6" s="13" t="inlineStr">
-        <is>
-          <t>上海农村商业银行股份有限公司2023年度企业级数据仓库和数据模型系统增选开发维护服务（C模式）框架</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>Hadoop</t>
-        </is>
-      </c>
-      <c r="C6" s="13" t="inlineStr">
-        <is>
-          <t>CDP</t>
-        </is>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>27</v>
-      </c>
-      <c r="E6" s="13" t="inlineStr">
-        <is>
-          <t>cloudera</t>
-        </is>
-      </c>
-      <c r="F6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="H6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K6" s="13" t="inlineStr">
-        <is>
-          <t>erwin</t>
-        </is>
-      </c>
-      <c r="L6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="N6" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A6" s="13" t="n"/>
+      <c r="B6" s="13" t="n"/>
+      <c r="C6" s="13" t="n"/>
+      <c r="D6" s="13" t="n"/>
+      <c r="E6" s="13" t="n"/>
+      <c r="F6" s="13" t="n"/>
+      <c r="G6" s="13" t="n"/>
+      <c r="H6" s="13" t="n"/>
+      <c r="I6" s="13" t="n"/>
+      <c r="J6" s="13" t="n"/>
+      <c r="K6" s="13" t="n"/>
+      <c r="L6" s="13" t="n"/>
+      <c r="M6" s="13" t="n"/>
+      <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
-      <c r="P6" s="13" t="inlineStr">
-        <is>
-          <t>监管报送，管理驾驶舱</t>
-        </is>
-      </c>
-      <c r="Q6" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R6" s="14" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="S6" s="13" t="inlineStr">
-        <is>
-          <t>CDP</t>
-        </is>
-      </c>
-      <c r="T6" s="13" t="inlineStr">
-        <is>
-          <t>2022.1-2023.12</t>
-        </is>
-      </c>
-      <c r="U6" s="13" t="inlineStr">
-        <is>
-          <t>并行阶段</t>
-        </is>
-      </c>
-      <c r="V6" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="P6" s="13" t="n"/>
+      <c r="Q6" s="14" t="n"/>
+      <c r="R6" s="14" t="n"/>
+      <c r="S6" s="13" t="n"/>
+      <c r="T6" s="13" t="n"/>
+      <c r="U6" s="13" t="n"/>
+      <c r="V6" s="13" t="n"/>
     </row>
     <row r="7" ht="15" customHeight="1" s="59">
-      <c r="A7" s="28" t="inlineStr">
-        <is>
-          <t>东亚银行标签平台</t>
-        </is>
-      </c>
-      <c r="B7" s="13" t="inlineStr">
-        <is>
-          <t>MPP</t>
-        </is>
-      </c>
-      <c r="C7" s="13" t="inlineStr">
-        <is>
-          <t>argodb</t>
-        </is>
-      </c>
-      <c r="D7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="H7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M7" s="13" t="inlineStr">
-        <is>
-          <t>麒麟V10</t>
-        </is>
-      </c>
-      <c r="N7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A7" s="28" t="n"/>
+      <c r="B7" s="13" t="n"/>
+      <c r="C7" s="13" t="n"/>
+      <c r="D7" s="13" t="n"/>
+      <c r="E7" s="13" t="n"/>
+      <c r="F7" s="13" t="n"/>
+      <c r="G7" s="13" t="n"/>
+      <c r="H7" s="13" t="n"/>
+      <c r="I7" s="13" t="n"/>
+      <c r="J7" s="13" t="n"/>
+      <c r="K7" s="13" t="n"/>
+      <c r="L7" s="13" t="n"/>
+      <c r="M7" s="13" t="n"/>
+      <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
-      <c r="P7" s="13" t="inlineStr">
-        <is>
-          <t>营销平台，crm</t>
-        </is>
-      </c>
-      <c r="Q7" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R7" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="S7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="P7" s="13" t="n"/>
+      <c r="Q7" s="13" t="n"/>
+      <c r="R7" s="13" t="n"/>
+      <c r="S7" s="13" t="n"/>
+      <c r="T7" s="13" t="n"/>
+      <c r="U7" s="13" t="n"/>
+      <c r="V7" s="13" t="n"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="59">
-      <c r="A8" s="28" t="inlineStr">
-        <is>
-          <t>东莞银行数据治理项目</t>
-        </is>
-      </c>
-      <c r="B8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="H8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="N8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A8" s="28" t="n"/>
+      <c r="B8" s="13" t="n"/>
+      <c r="C8" s="13" t="n"/>
+      <c r="D8" s="13" t="n"/>
+      <c r="E8" s="13" t="n"/>
+      <c r="F8" s="13" t="n"/>
+      <c r="G8" s="13" t="n"/>
+      <c r="H8" s="13" t="n"/>
+      <c r="I8" s="13" t="n"/>
+      <c r="J8" s="13" t="n"/>
+      <c r="K8" s="13" t="n"/>
+      <c r="L8" s="13" t="n"/>
+      <c r="M8" s="13" t="n"/>
+      <c r="N8" s="13" t="n"/>
       <c r="O8" s="13" t="n"/>
-      <c r="P8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="S8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="P8" s="13" t="n"/>
+      <c r="Q8" s="13" t="n"/>
+      <c r="R8" s="13" t="n"/>
+      <c r="S8" s="13" t="n"/>
+      <c r="T8" s="13" t="n"/>
+      <c r="U8" s="13" t="n"/>
+      <c r="V8" s="13" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1" s="59">
-      <c r="A9" s="28" t="inlineStr">
-        <is>
-          <t>中信财务数据治理和数据中台建设项目</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>Oracle</t>
-        </is>
-      </c>
-      <c r="C9" s="13" t="inlineStr">
-        <is>
-          <t>19C</t>
-        </is>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F9" s="13" t="inlineStr">
-        <is>
-          <t>SmartBI</t>
-        </is>
-      </c>
-      <c r="G9" s="13" t="inlineStr">
-        <is>
-          <t>长亮科技企业级调度平台v8.0</t>
-        </is>
-      </c>
-      <c r="H9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I9" s="13" t="inlineStr">
-        <is>
-          <t>长亮科技数据交换平台v5.5</t>
-        </is>
-      </c>
-      <c r="J9" s="13" t="inlineStr">
-        <is>
-          <t>长亮科技数据资产管理平台v5.0</t>
-        </is>
-      </c>
-      <c r="K9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L9" s="13" t="inlineStr">
-        <is>
-          <t>阿里云ECS</t>
-        </is>
-      </c>
-      <c r="M9" s="13" t="inlineStr">
-        <is>
-          <t>ubantu 22</t>
-        </is>
-      </c>
-      <c r="N9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A9" s="28" t="n"/>
+      <c r="B9" s="13" t="n"/>
+      <c r="C9" s="13" t="n"/>
+      <c r="D9" s="13" t="n"/>
+      <c r="E9" s="13" t="n"/>
+      <c r="F9" s="13" t="n"/>
+      <c r="G9" s="13" t="n"/>
+      <c r="H9" s="13" t="n"/>
+      <c r="I9" s="13" t="n"/>
+      <c r="J9" s="13" t="n"/>
+      <c r="K9" s="13" t="n"/>
+      <c r="L9" s="13" t="n"/>
+      <c r="M9" s="13" t="n"/>
+      <c r="N9" s="13" t="n"/>
       <c r="O9" s="13" t="n"/>
-      <c r="P9" s="13" t="inlineStr">
-        <is>
-          <t>监管报送，流动性管理系统，管理驾驶舱</t>
-        </is>
-      </c>
-      <c r="Q9" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R9" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="S9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V9" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="P9" s="13" t="n"/>
+      <c r="Q9" s="13" t="n"/>
+      <c r="R9" s="13" t="n"/>
+      <c r="S9" s="13" t="n"/>
+      <c r="T9" s="13" t="n"/>
+      <c r="U9" s="13" t="n"/>
+      <c r="V9" s="13" t="n"/>
     </row>
     <row r="10" ht="15" customFormat="1" customHeight="1" s="31">
-      <c r="A10" s="32" t="inlineStr">
-        <is>
-          <t>中化财务数据平台2023年优化升级项目</t>
-        </is>
-      </c>
-      <c r="B10" s="14" t="inlineStr">
-        <is>
-          <t>MPP</t>
-        </is>
-      </c>
-      <c r="C10" s="14" t="inlineStr">
-        <is>
-          <t>Oracle 11.2.0.4.0</t>
-        </is>
-      </c>
-      <c r="D10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F10" s="14" t="inlineStr">
-        <is>
-          <t>SmartBI</t>
-        </is>
-      </c>
-      <c r="G10" s="14" t="inlineStr">
-        <is>
-          <t>长亮科技企业级调度平台v2.0</t>
-        </is>
-      </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K10" s="14" t="inlineStr">
-        <is>
-          <t>自主研发</t>
-        </is>
-      </c>
-      <c r="L10" s="14" t="inlineStr">
-        <is>
-          <t>centos 7.4</t>
-        </is>
-      </c>
-      <c r="M10" s="14" t="inlineStr">
-        <is>
-          <t>windows10</t>
-        </is>
-      </c>
-      <c r="N10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A10" s="32" t="n"/>
+      <c r="B10" s="14" t="n"/>
+      <c r="C10" s="14" t="n"/>
+      <c r="D10" s="14" t="n"/>
+      <c r="E10" s="14" t="n"/>
+      <c r="F10" s="14" t="n"/>
+      <c r="G10" s="14" t="n"/>
+      <c r="H10" s="14" t="n"/>
+      <c r="I10" s="14" t="n"/>
+      <c r="J10" s="14" t="n"/>
+      <c r="K10" s="14" t="n"/>
+      <c r="L10" s="14" t="n"/>
+      <c r="M10" s="14" t="n"/>
+      <c r="N10" s="14" t="n"/>
       <c r="O10" s="14" t="n"/>
-      <c r="P10" s="14" t="inlineStr">
-        <is>
-          <t>监管报送，管理驾驶舱</t>
-        </is>
-      </c>
-      <c r="Q10" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R10" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="S10" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T10" s="37" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U10" s="37" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V10" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="P10" s="14" t="n"/>
+      <c r="Q10" s="14" t="n"/>
+      <c r="R10" s="14" t="n"/>
+      <c r="S10" s="14" t="n"/>
+      <c r="T10" s="37" t="n"/>
+      <c r="U10" s="37" t="n"/>
+      <c r="V10" s="14" t="n"/>
     </row>
     <row r="11" ht="15" customFormat="1" customHeight="1" s="31">
-      <c r="A11" s="14" t="inlineStr">
-        <is>
-          <t>中国银行应用软件支持服务（MUREX）项目</t>
-        </is>
-      </c>
-      <c r="B11" s="14" t="inlineStr">
-        <is>
-          <t>ORACLE</t>
-        </is>
-      </c>
-      <c r="C11" s="14" t="inlineStr">
-        <is>
-          <t>11G</t>
-        </is>
-      </c>
-      <c r="D11" s="14" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="H11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L11" s="14" t="inlineStr">
-        <is>
-          <t>PC SERVER</t>
-        </is>
-      </c>
-      <c r="M11" s="14" t="inlineStr">
-        <is>
-          <t>RHEL6.6 x86-64</t>
-        </is>
-      </c>
-      <c r="N11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="14" t="n"/>
+      <c r="C11" s="14" t="n"/>
+      <c r="D11" s="14" t="n"/>
+      <c r="E11" s="14" t="n"/>
+      <c r="F11" s="14" t="n"/>
+      <c r="G11" s="14" t="n"/>
+      <c r="H11" s="14" t="n"/>
+      <c r="I11" s="14" t="n"/>
+      <c r="J11" s="14" t="n"/>
+      <c r="K11" s="14" t="n"/>
+      <c r="L11" s="14" t="n"/>
+      <c r="M11" s="14" t="n"/>
+      <c r="N11" s="14" t="n"/>
       <c r="O11" s="14" t="n"/>
-      <c r="P11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="Q11" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R11" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="S11" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T11" s="37" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U11" s="37" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V11" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="P11" s="14" t="n"/>
+      <c r="Q11" s="14" t="n"/>
+      <c r="R11" s="14" t="n"/>
+      <c r="S11" s="14" t="n"/>
+      <c r="T11" s="37" t="n"/>
+      <c r="U11" s="37" t="n"/>
+      <c r="V11" s="14" t="n"/>
     </row>
     <row r="12" ht="15" customHeight="1" s="59">
-      <c r="A12" s="14" t="inlineStr">
-        <is>
-          <t>中国银行股份有限公司银行卡数据运营服务项目</t>
-        </is>
-      </c>
-      <c r="B12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="H12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="I12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="J12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="K12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="L12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="N12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A12" s="14" t="n"/>
+      <c r="B12" s="13" t="n"/>
+      <c r="C12" s="13" t="n"/>
+      <c r="D12" s="13" t="n"/>
+      <c r="E12" s="13" t="n"/>
+      <c r="F12" s="13" t="n"/>
+      <c r="G12" s="13" t="n"/>
+      <c r="H12" s="13" t="n"/>
+      <c r="I12" s="13" t="n"/>
+      <c r="J12" s="13" t="n"/>
+      <c r="K12" s="13" t="n"/>
+      <c r="L12" s="13" t="n"/>
+      <c r="M12" s="13" t="n"/>
+      <c r="N12" s="13" t="n"/>
       <c r="O12" s="13" t="n"/>
-      <c r="P12" s="14" t="inlineStr">
-        <is>
-          <t>评分卡、一表通、EAST、1104、RDA</t>
-        </is>
-      </c>
-      <c r="Q12" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R12" s="13" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="S12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="T12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="U12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="V12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="P12" s="14" t="n"/>
+      <c r="Q12" s="13" t="n"/>
+      <c r="R12" s="13" t="n"/>
+      <c r="S12" s="13" t="n"/>
+      <c r="T12" s="13" t="n"/>
+      <c r="U12" s="13" t="n"/>
+      <c r="V12" s="13" t="n"/>
     </row>
     <row r="13" ht="15" customFormat="1" customHeight="1" s="31">
-      <c r="A13" s="14" t="inlineStr">
-        <is>
-          <t>红塔银行数据中台项目</t>
-        </is>
-      </c>
-      <c r="B13" s="14" t="inlineStr">
-        <is>
-          <t>MPP</t>
-        </is>
-      </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>Maxcompute</t>
-        </is>
-      </c>
-      <c r="D13" s="14" t="n">
-        <v>10</v>
-      </c>
-      <c r="E13" s="14" t="inlineStr">
-        <is>
-          <t>阿里云</t>
-        </is>
-      </c>
-      <c r="F13" s="14" t="inlineStr">
-        <is>
-          <t>帆软BI</t>
-        </is>
-      </c>
-      <c r="G13" s="14" t="inlineStr">
-        <is>
-          <t>dataworks</t>
-        </is>
-      </c>
-      <c r="H13" s="14" t="inlineStr">
-        <is>
-          <t>dataworks</t>
-        </is>
-      </c>
-      <c r="I13" s="14" t="inlineStr">
-        <is>
-          <t>长亮科技数据交换平台v2.0</t>
-        </is>
-      </c>
-      <c r="J13" s="14" t="inlineStr">
-        <is>
-          <t>神马</t>
-        </is>
-      </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>阿里云</t>
-        </is>
-      </c>
-      <c r="L13" s="14" t="inlineStr">
-        <is>
-          <t>阿里云</t>
-        </is>
-      </c>
-      <c r="M13" s="14" t="inlineStr">
-        <is>
-          <t>麒麟V10</t>
-        </is>
-      </c>
-      <c r="N13" s="14" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A13" s="14" t="n"/>
+      <c r="B13" s="14" t="n"/>
+      <c r="C13" s="14" t="n"/>
+      <c r="D13" s="14" t="n"/>
+      <c r="E13" s="14" t="n"/>
+      <c r="F13" s="14" t="n"/>
+      <c r="G13" s="14" t="n"/>
+      <c r="H13" s="14" t="n"/>
+      <c r="I13" s="14" t="n"/>
+      <c r="J13" s="14" t="n"/>
+      <c r="K13" s="14" t="n"/>
+      <c r="L13" s="14" t="n"/>
+      <c r="M13" s="14" t="n"/>
+      <c r="N13" s="14" t="n"/>
       <c r="O13" s="14" t="n"/>
-      <c r="P13" s="14" t="inlineStr">
-        <is>
-          <t>监管报送，管理驾驶舱</t>
-        </is>
-      </c>
-      <c r="Q13" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="R13" s="14" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="S13" s="14" t="inlineStr">
-        <is>
-          <t>Maxcompute</t>
-        </is>
-      </c>
-      <c r="T13" s="37" t="inlineStr">
-        <is>
-          <t>2023.11-2024.12</t>
-        </is>
-      </c>
-      <c r="U13" s="37" t="inlineStr">
-        <is>
-          <t>需求分析</t>
-        </is>
-      </c>
-      <c r="V13" s="14" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
+      <c r="P13" s="14" t="n"/>
+      <c r="Q13" s="14" t="n"/>
+      <c r="R13" s="14" t="n"/>
+      <c r="S13" s="14" t="n"/>
+      <c r="T13" s="37" t="n"/>
+      <c r="U13" s="37" t="n"/>
+      <c r="V13" s="14" t="n"/>
     </row>
     <row r="14" ht="15" customHeight="1" s="59">
       <c r="A14" s="13" t="n"/>
@@ -6830,8 +4898,8 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="P2:R2"/>
     <mergeCell ref="B2:O2"/>
-    <mergeCell ref="P2:R2"/>
     <mergeCell ref="S2:U2"/>
   </mergeCells>
   <hyperlinks>
@@ -6936,7 +5004,7 @@
     <row r="4" ht="15" customFormat="1" customHeight="1" s="19">
       <c r="A4" s="26" t="inlineStr">
         <is>
-          <t>企业级数据仓库迁移项目（二期）项目</t>
+          <t>xxxxxx</t>
         </is>
       </c>
       <c r="B4" s="26" t="inlineStr">
@@ -6961,350 +5029,104 @@
       </c>
       <c r="F4" s="26" t="inlineStr">
         <is>
-          <t>数据仓库</t>
+          <t>/</t>
         </is>
       </c>
       <c r="G4" s="26" t="inlineStr">
         <is>
-          <t>Teradata</t>
+          <t>xxxxx-xxxxx</t>
         </is>
       </c>
       <c r="H4" s="26" t="n"/>
     </row>
     <row r="5" ht="15" customFormat="1" customHeight="1" s="20">
-      <c r="A5" s="27" t="inlineStr">
-        <is>
-          <t>上海农商行2023年度内部评级系统、风险加权资产计量系统（C模式）框架协议（2023.3.24-2024.6.30）-2023年结算</t>
-        </is>
-      </c>
-      <c r="B5" s="27" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C5" s="27" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D5" s="27" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E5" s="27" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F5" s="27" t="inlineStr">
-        <is>
-          <t>ODS</t>
-        </is>
-      </c>
-      <c r="G5" s="27" t="inlineStr">
-        <is>
-          <t>安硕</t>
-        </is>
-      </c>
+      <c r="A5" s="27" t="n"/>
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="27" t="n"/>
+      <c r="D5" s="27" t="n"/>
+      <c r="E5" s="27" t="n"/>
+      <c r="F5" s="27" t="n"/>
+      <c r="G5" s="27" t="n"/>
       <c r="H5" s="27" t="n"/>
     </row>
     <row r="6" ht="15" customFormat="1" customHeight="1" s="19">
-      <c r="A6" s="28" t="inlineStr">
-        <is>
-          <t>上海农村商业银行股份有限公司2023年度企业级数据仓库和数据模型系统增选开发维护服务（C模式）框架</t>
-        </is>
-      </c>
-      <c r="B6" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C6" s="26" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="D6" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E6" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F6" s="26" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="G6" s="26" t="inlineStr">
-        <is>
-          <t>TD</t>
-        </is>
-      </c>
+      <c r="A6" s="28" t="n"/>
+      <c r="B6" s="26" t="n"/>
+      <c r="C6" s="26" t="n"/>
+      <c r="D6" s="26" t="n"/>
+      <c r="E6" s="26" t="n"/>
+      <c r="F6" s="26" t="n"/>
+      <c r="G6" s="26" t="n"/>
       <c r="H6" s="26" t="n"/>
     </row>
     <row r="7" ht="15" customHeight="1" s="59">
-      <c r="A7" s="28" t="inlineStr">
-        <is>
-          <t>东亚银行标签平台</t>
-        </is>
-      </c>
-      <c r="B7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F7" s="13" t="inlineStr">
-        <is>
-          <t>大数据平台</t>
-        </is>
-      </c>
-      <c r="G7" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A7" s="28" t="n"/>
+      <c r="B7" s="13" t="n"/>
+      <c r="C7" s="13" t="n"/>
+      <c r="D7" s="13" t="n"/>
+      <c r="E7" s="13" t="n"/>
+      <c r="F7" s="13" t="n"/>
+      <c r="G7" s="13" t="n"/>
       <c r="H7" s="13" t="n"/>
     </row>
     <row r="8" ht="15" customHeight="1" s="59">
-      <c r="A8" s="28" t="inlineStr">
-        <is>
-          <t>东莞银行数据治理项目</t>
-        </is>
-      </c>
-      <c r="B8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G8" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A8" s="28" t="n"/>
+      <c r="B8" s="13" t="n"/>
+      <c r="C8" s="13" t="n"/>
+      <c r="D8" s="13" t="n"/>
+      <c r="E8" s="13" t="n"/>
+      <c r="F8" s="13" t="n"/>
+      <c r="G8" s="13" t="n"/>
       <c r="H8" s="13" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1" s="59">
-      <c r="A9" s="26" t="inlineStr">
-        <is>
-          <t>中信财务数据治理和数据中台建设项目</t>
-        </is>
-      </c>
-      <c r="B9" s="13" t="inlineStr">
-        <is>
-          <t>SmartBI</t>
-        </is>
-      </c>
-      <c r="C9" s="13" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="inlineStr">
-        <is>
-          <t>Oracle</t>
-        </is>
-      </c>
-      <c r="F9" s="13" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="G9" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A9" s="26" t="n"/>
+      <c r="B9" s="13" t="n"/>
+      <c r="C9" s="13" t="n"/>
+      <c r="D9" s="13" t="n"/>
+      <c r="E9" s="13" t="n"/>
+      <c r="F9" s="13" t="n"/>
+      <c r="G9" s="13" t="n"/>
       <c r="H9" s="13" t="n"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="59">
-      <c r="A10" s="26" t="inlineStr">
-        <is>
-          <t>中化财务数据平台2023年优化升级项目</t>
-        </is>
-      </c>
-      <c r="B10" s="26" t="inlineStr">
-        <is>
-          <t>SmartBI</t>
-        </is>
-      </c>
-      <c r="C10" s="26" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="D10" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="26" t="inlineStr">
-        <is>
-          <t>Oracle</t>
-        </is>
-      </c>
-      <c r="F10" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="G10" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A10" s="26" t="n"/>
+      <c r="B10" s="26" t="n"/>
+      <c r="C10" s="26" t="n"/>
+      <c r="D10" s="26" t="n"/>
+      <c r="E10" s="26" t="n"/>
+      <c r="F10" s="26" t="n"/>
+      <c r="G10" s="26" t="n"/>
       <c r="H10" s="26" t="n"/>
     </row>
     <row r="11" ht="15" customFormat="1" customHeight="1" s="19">
-      <c r="A11" s="26" t="inlineStr">
-        <is>
-          <t>中国银行应用软件支持服务（MUREX）项目</t>
-        </is>
-      </c>
-      <c r="B11" s="26" t="inlineStr">
-        <is>
-          <t>Datamart</t>
-        </is>
-      </c>
-      <c r="C11" s="26" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="D11" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E11" s="26" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F11" s="26" t="inlineStr">
-        <is>
-          <t>外部导入，手工簿记</t>
-        </is>
-      </c>
-      <c r="G11" s="26" t="inlineStr">
-        <is>
-          <t>易九州</t>
-        </is>
-      </c>
+      <c r="A11" s="26" t="n"/>
+      <c r="B11" s="26" t="n"/>
+      <c r="C11" s="26" t="n"/>
+      <c r="D11" s="26" t="n"/>
+      <c r="E11" s="26" t="n"/>
+      <c r="F11" s="26" t="n"/>
+      <c r="G11" s="26" t="n"/>
       <c r="H11" s="26" t="n"/>
     </row>
     <row r="12" ht="15" customHeight="1" s="59">
-      <c r="A12" s="13" t="inlineStr">
-        <is>
-          <t>中国银行股份有限公司银行卡数据运营服务项目</t>
-        </is>
-      </c>
-      <c r="B12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="C12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F12" s="13" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="G12" s="13" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
+      <c r="A12" s="13" t="n"/>
+      <c r="B12" s="13" t="n"/>
+      <c r="C12" s="13" t="n"/>
+      <c r="D12" s="13" t="n"/>
+      <c r="E12" s="13" t="n"/>
+      <c r="F12" s="13" t="n"/>
+      <c r="G12" s="13" t="n"/>
       <c r="H12" s="13" t="n"/>
     </row>
     <row r="13" ht="15" customFormat="1" customHeight="1" s="1">
-      <c r="A13" s="26" t="inlineStr">
-        <is>
-          <t>红塔银行数据中台项目</t>
-        </is>
-      </c>
-      <c r="B13" s="27" t="inlineStr">
-        <is>
-          <t>帆软BI</t>
-        </is>
-      </c>
-      <c r="C13" s="27" t="inlineStr">
-        <is>
-          <t>否</t>
-        </is>
-      </c>
-      <c r="D13" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="27" t="inlineStr">
-        <is>
-          <t>Oracle</t>
-        </is>
-      </c>
-      <c r="F13" s="27" t="inlineStr">
-        <is>
-          <t>数据仓库</t>
-        </is>
-      </c>
-      <c r="G13" s="27" t="inlineStr">
-        <is>
-          <t>先数</t>
-        </is>
-      </c>
+      <c r="A13" s="26" t="n"/>
+      <c r="B13" s="27" t="n"/>
+      <c r="C13" s="27" t="n"/>
+      <c r="D13" s="27" t="n"/>
+      <c r="E13" s="27" t="n"/>
+      <c r="F13" s="27" t="n"/>
+      <c r="G13" s="27" t="n"/>
       <c r="H13" s="27" t="n"/>
     </row>
     <row r="14" ht="15" customHeight="1" s="59">
@@ -7851,8 +5673,8 @@
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="A4">
     <cfRule type="expression" priority="4" dxfId="0">
@@ -8710,7 +6532,7 @@
     <row r="64" ht="15" customHeight="1" s="59"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="F2:F3" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="F2:F3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"北京市,上海市,天津市,重庆市,黑龙江省,辽宁省,吉林省,河北省,河南省,湖北省,湖南省,山东省,山西省,陕西省,安徽省,浙江省,江苏省,福建省,广东省,海南省,四川省,云南省,贵州省,青海省,甘肃省,江西省,台湾省,内蒙古自治区,宁夏回族自治区,新疆维吾尔自治区,西藏自治区,广西壮族自治区,香港特别行政区、澳门特别行政区,香港特别行政区、澳门特别行政区"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8720,7 +6542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet5">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9318,7 +7140,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10357,22 +8179,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A4:A15"/>
+    <mergeCell ref="B56:B68"/>
+    <mergeCell ref="B88:B100"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B18:B26"/>
+    <mergeCell ref="B74:B87"/>
+    <mergeCell ref="A56:A100"/>
+    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="B4:B10"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A15"/>
-    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A101:B103"/>
+    <mergeCell ref="B69:B73"/>
     <mergeCell ref="A27:A55"/>
-    <mergeCell ref="A56:A100"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B26"/>
     <mergeCell ref="B27:B48"/>
-    <mergeCell ref="A101:B103"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="B56:B68"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="B74:B87"/>
-    <mergeCell ref="B88:B100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>